<commit_message>
Added period to KPIs
</commit_message>
<xml_diff>
--- a/public/sample_uploads/kpis.xlsx
+++ b/public/sample_uploads/kpis.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thimmaiah\work\IRM\public\sample_uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAB45B20-955D-42B6-801C-CF57A30FE860}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4230E98F-AC77-45FE-A4E5-4A2B8F868FA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>Name</t>
   </si>
@@ -49,6 +49,15 @@
   </si>
   <si>
     <t>Num of Stores</t>
+  </si>
+  <si>
+    <t>Period</t>
+  </si>
+  <si>
+    <t>Quarter</t>
+  </si>
+  <si>
+    <t>Annual</t>
   </si>
 </sst>
 </file>
@@ -367,73 +376,89 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="11.9296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.9296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.9296875" customWidth="1"/>
+    <col min="4" max="4" width="9.9296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2">
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2">
         <v>1000</v>
       </c>
-      <c r="C2" s="1">
+      <c r="D2" s="1">
         <v>44927</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3">
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3">
         <v>500</v>
       </c>
-      <c r="C3" s="1">
+      <c r="D3" s="1">
         <v>44927</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B4">
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4">
         <v>400</v>
       </c>
-      <c r="C4" s="1">
+      <c r="D4" s="1">
         <v>44927</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="B5">
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5">
         <v>3</v>
       </c>
-      <c r="C5" s="1">
+      <c r="D5" s="1">
         <v>44927</v>
       </c>
     </row>

</xml_diff>